<commit_message>
Reducing memory consumption (#11)
* checking memmory usage

* replacement of sklearn for ANN Normalization layer

* cleaning unused data after a session
</commit_message>
<xml_diff>
--- a/cs_app/data/df_n_impervious.xlsx
+++ b/cs_app/data/df_n_impervious.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,23 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>runoff</t>
-  </si>
-  <si>
-    <t>peak_runoff_rate</t>
-  </si>
-  <si>
-    <t>infiltration</t>
-  </si>
-  <si>
-    <t>evaporation</t>
   </si>
   <si>
     <t>N-Imperv</t>
@@ -34,8 +25,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,17 +85,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +138,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +172,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +207,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,327 +383,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1707.2395553775641</v>
       </c>
       <c r="B2">
-        <v>1707.239555377564</v>
-      </c>
-      <c r="C2">
-        <v>1.015679722108064</v>
-      </c>
-      <c r="D2">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0.011</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>1</v>
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1707.1214101181599</v>
       </c>
       <c r="B3">
-        <v>1707.12141011816</v>
-      </c>
-      <c r="C3">
-        <v>1.015671761891542</v>
-      </c>
-      <c r="D3">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1">
-        <v>2</v>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1707.0154638144959</v>
       </c>
       <c r="B4">
-        <v>1707.015463814496</v>
-      </c>
-      <c r="C4">
-        <v>1.015659378820929</v>
-      </c>
-      <c r="D4">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>3</v>
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1706.919458513222</v>
       </c>
       <c r="B5">
-        <v>1706.919458513222</v>
-      </c>
-      <c r="C5">
-        <v>1.01564119086132</v>
-      </c>
-      <c r="D5">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0.014</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1">
-        <v>4</v>
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1706.8316628723501</v>
       </c>
       <c r="B6">
-        <v>1706.83166287235</v>
-      </c>
-      <c r="C6">
-        <v>1.015615699402178</v>
-      </c>
-      <c r="D6">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0.015</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>5</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1706.255565308622</v>
       </c>
       <c r="B7">
-        <v>1706.255565308622</v>
-      </c>
-      <c r="C7">
-        <v>1.014798432165925</v>
-      </c>
-      <c r="D7">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0.024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>6</v>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1705.2329458801501</v>
       </c>
       <c r="B8">
-        <v>1705.23294588015</v>
-      </c>
-      <c r="C8">
-        <v>1.001681583322129</v>
-      </c>
-      <c r="D8">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1704.892365627999</v>
       </c>
       <c r="B9">
-        <v>1704.892365627999</v>
-      </c>
-      <c r="C9">
-        <v>0.99221304442491</v>
-      </c>
-      <c r="D9">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1702.379488620785</v>
       </c>
       <c r="B10">
-        <v>1702.379488620785</v>
-      </c>
-      <c r="C10">
-        <v>0.8955705622113455</v>
-      </c>
-      <c r="D10">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1701.5821946323281</v>
       </c>
       <c r="B11">
-        <v>1701.582194632328</v>
-      </c>
-      <c r="C11">
-        <v>0.8660485406317805</v>
-      </c>
-      <c r="D11">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1700.748064144449</v>
       </c>
       <c r="B12">
-        <v>1700.748064144449</v>
-      </c>
-      <c r="C12">
-        <v>0.8374962114405451</v>
-      </c>
-      <c r="D12">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
         <v>0.17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1697.5605483398731</v>
       </c>
       <c r="B13">
-        <v>1697.560548339873</v>
-      </c>
-      <c r="C13">
-        <v>0.748479264258672</v>
-      </c>
-      <c r="D13">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
         <v>0.24</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1689.0028244700859</v>
       </c>
       <c r="B14">
-        <v>1689.002824470086</v>
-      </c>
-      <c r="C14">
-        <v>0.6046034721027908</v>
-      </c>
-      <c r="D14">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1688.420178896876</v>
       </c>
       <c r="B15">
-        <v>1688.420178896876</v>
-      </c>
-      <c r="C15">
-        <v>0.5977281690577967</v>
-      </c>
-      <c r="D15">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
         <v>0.41</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>14</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1662.818432752422</v>
       </c>
       <c r="B16">
-        <v>1662.818432752422</v>
-      </c>
-      <c r="C16">
-        <v>0.4301227664510335</v>
-      </c>
-      <c r="D16">
-        <v>6531.097978622704</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
         <v>0.8</v>
       </c>
     </row>

</xml_diff>